<commit_message>
Managed to move period but not keep original
</commit_message>
<xml_diff>
--- a/Schedules/AV_course_schedule.xlsx
+++ b/Schedules/AV_course_schedule.xlsx
@@ -130,8 +130,7 @@
 AM-340L-12802-Moon-IDE-317</t>
   </si>
   <si>
-    <t>5
-AM-201-05816-Balch-EAX-011
+    <t>7
 AT-410L-05804-Adelizzi-EAX-022
 AT-410L-05804-Adelizzi-EAX-023</t>
   </si>
@@ -594,7 +593,7 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
@@ -614,7 +613,7 @@
         <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Made double blocks work
</commit_message>
<xml_diff>
--- a/Schedules/AV_course_schedule.xlsx
+++ b/Schedules/AV_course_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>TIME</t>
   </si>
@@ -128,6 +128,12 @@
   <si>
     <t>12
 AM-340L-12802-Moon-IDE-317</t>
+  </si>
+  <si>
+    <t>5
+AM-201-05816-Balch-EAX-011
+AT-410L-05804-Adelizzi-EAX-022
+AT-410L-05804-Adelizzi-EAX-023</t>
   </si>
   <si>
     <t>7
@@ -556,7 +562,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -576,7 +582,7 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -593,10 +599,10 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -613,10 +619,10 @@
         <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -636,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -656,7 +662,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -676,7 +682,7 @@
         <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -696,7 +702,7 @@
         <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -716,7 +722,7 @@
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the nan and float issue in friday column
</commit_message>
<xml_diff>
--- a/Schedules/AV_course_schedule.xlsx
+++ b/Schedules/AV_course_schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>TIME</t>
   </si>
@@ -141,27 +141,7 @@
 AT-410L-05804-Adelizzi-EAX-023</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>4.0
-AV-306-04805-Breuder-EAX-009</t>
-  </si>
-  <si>
-    <t>6.0</t>
-  </si>
-  <si>
-    <t>8.0
-AV-205-08815-LaFauci-IDE-209</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>nan</t>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -562,7 +542,7 @@
         <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -582,7 +562,7 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -602,7 +582,7 @@
         <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -622,7 +602,7 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -642,7 +622,7 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -662,7 +642,7 @@
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -681,9 +661,6 @@
       <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -701,9 +678,6 @@
       <c r="E9" t="s">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
@@ -720,9 +694,6 @@
       </c>
       <c r="E10" t="s">
         <v>31</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>